<commit_message>
adding signin working files
</commit_message>
<xml_diff>
--- a/src/test/resources/excelTestData/signInTestData.xlsx
+++ b/src/test/resources/excelTestData/signInTestData.xlsx
@@ -1,34 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{CF061EF3-625E-46B0-82FD-63B5F4E640EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="20700" windowHeight="12300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="login_valid" sheetId="1" r:id="rId1"/>
-    <sheet name="login_invalid" sheetId="2" r:id="rId2"/>
+    <sheet state="visible" name="login_valid" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="login_invalid" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:F21"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
-  <si>
-    <t>Scenarioname</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>message</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+  <si>
+    <t>ScenarioName</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
   <si>
     <t>valid username and valid password</t>
@@ -40,39 +32,21 @@
     <t>testers123</t>
   </si>
   <si>
+    <t>ExpectedErrMsg</t>
+  </si>
+  <si>
     <t>You are logged in</t>
   </si>
   <si>
-    <t>dsalgo231</t>
-  </si>
-  <si>
-    <t>automation2025#</t>
-  </si>
-  <si>
-    <t>ScenarioName</t>
-  </si>
-  <si>
-    <t>expectedErrMsg</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
     <t>Empty username and empty password</t>
   </si>
   <si>
     <t>Please fill out this field.</t>
   </si>
   <si>
-    <t>Username</t>
-  </si>
-  <si>
     <t>Valid username and empty password</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
     <t>Empty username and valid password</t>
   </si>
   <si>
@@ -94,78 +68,106 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="5">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="&quot;Consolas&quot;"/>
+      <sz val="12.0"/>
+      <color rgb="FF004085"/>
+      <name val="-apple-system"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD4D4D4"/>
-        <bgColor rgb="FFD4D4D4"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCE5FF"/>
+        <bgColor rgb="FFCCE5FF"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+  <cellXfs count="10">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -355,177 +357,220 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="27.08984375" customWidth="1"/>
-    <col min="2" max="2" width="21.90625" customWidth="1"/>
-    <col min="3" max="3" width="15.6328125" customWidth="1"/>
-    <col min="4" max="4" width="27.36328125" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="39.63"/>
+    <col customWidth="1" min="2" max="2" width="21.88"/>
+    <col customWidth="1" min="3" max="3" width="15.63"/>
+    <col customWidth="1" min="4" max="4" width="27.38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="40.36328125" customWidth="1"/>
-    <col min="4" max="4" width="32.08984375" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="40.38"/>
+    <col customWidth="1" min="4" max="4" width="32.13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A1" s="3" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
+      <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="D7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>